<commit_message>
new version of dependency_rate
</commit_message>
<xml_diff>
--- a/data/Combined-data/Rente_All.xlsx
+++ b/data/Combined-data/Rente_All.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="German_pop" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Employment_Rate" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="NewRenter" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Immigration" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="LifeExpentency" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Fertility_per_women" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sheet5" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8672" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8677" uniqueCount="58">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -38,7 +40,7 @@
     <t xml:space="preserve">Age</t>
   </si>
   <si>
-    <t xml:space="preserve">PopCount</t>
+    <t xml:space="preserve">Population</t>
   </si>
   <si>
     <t xml:space="preserve">Germany</t>
@@ -143,7 +145,7 @@
     <t xml:space="preserve">Annual growth rate of total population</t>
   </si>
   <si>
-    <t xml:space="preserve">Employed_total</t>
+    <t xml:space="preserve">Employed</t>
   </si>
   <si>
     <t xml:space="preserve">Perct_Women</t>
@@ -185,10 +187,19 @@
     <t xml:space="preserve">Growth Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">LifeExpentency (year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fertility Rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">migration ref </t>
   </si>
   <si>
     <t xml:space="preserve">https://www.macrotrends.net/countries/DEU/germany/net-migration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=qP_vcYUfepA</t>
   </si>
 </sst>
 </file>
@@ -225,6 +236,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -316,11 +328,11 @@
   </sheetPr>
   <dimension ref="A1:H2884"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2760" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2777" activeCellId="0" sqref="D2777"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
@@ -49378,11 +49390,11 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
@@ -50408,7 +50420,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -51004,7 +51016,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -51385,20 +51397,579 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1990</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>75.227756097561</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>75.319512195122</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>75.819512195122</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>75.8707317073171</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1994</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>76.2707317073171</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>76.4219512195122</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1996</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>76.6731707317073</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>77.0731707317073</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1998</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>77.4756097560976</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>77.7268292682927</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>77.9268292682927</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>78.3292682926829</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>78.2292682926829</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>78.3804878048781</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>78.6804878048781</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>78.9317073170732</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>79.1317073170732</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>79.5341463414634</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>79.7365853658537</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>79.8365853658537</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>79.9878048780488</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>80.4365853658537</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>80.5390243902439</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>80.490243902439</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>81.090243902439</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>80.6414634146341</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>80.990243902439</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>80.9926829268293</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>80.8926829268293</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>80.9414634146342</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1990</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1991</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1992</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1993</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1994</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1996</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1998</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>